<commit_message>
JNG-647: support custom types
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
@@ -382,10 +382,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -871,9 +873,11 @@
         <v>48</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C34" s="4" t="n">
+        <v>1024</v>
+      </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">

</xml_diff>

<commit_message>
JNG-1085: fix date and timestamp types
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t xml:space="preserve">Judo</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">java.time.OffsetDateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIMESTAMP WITH TIMEZONE</t>
   </si>
   <si>
     <t xml:space="preserve">java.time.ZonedDateTime</t>
@@ -449,7 +452,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -463,7 +466,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -491,7 +494,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -499,21 +502,21 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -524,21 +527,21 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
@@ -547,141 +550,141 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="n">
@@ -691,71 +694,71 @@
         <v>0</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="3" t="n">
@@ -765,15 +768,15 @@
         <v>20</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>255</v>
@@ -781,99 +784,99 @@
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>4095</v>
@@ -881,7 +884,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
JNG-1596: add seek parameter for pagination, fix naming conflicts and UUID type name in hsqldb
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
   <si>
     <t xml:space="preserve">Judo</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve">byte[]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UUID</t>
   </si>
   <si>
     <t xml:space="preserve">java.sql.Blob</t>
@@ -378,7 +375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -388,7 +385,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="21.9"/>
@@ -908,9 +905,11 @@
         <v>45</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>36</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
@@ -922,12 +921,14 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>36</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
@@ -939,12 +940,14 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <v>36</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
@@ -956,12 +959,14 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <v>36</v>
+      </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
@@ -973,7 +978,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
JNG-2588: asm2rdbms - update fillType method and data type excels to handle maxLength, precision and scale provided as constraints
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t xml:space="preserve">Judo</t>
   </si>
@@ -121,6 +121,9 @@
     <t xml:space="preserve">DECIMAL</t>
   </si>
   <si>
+    <t xml:space="preserve">#contraints:precision</t>
+  </si>
+  <si>
     <t xml:space="preserve">float</t>
   </si>
   <si>
@@ -142,10 +145,16 @@
     <t xml:space="preserve">java.math.BigDecimal</t>
   </si>
   <si>
+    <t xml:space="preserve">#contraints:scale</t>
+  </si>
+  <si>
     <t xml:space="preserve">java.lang.String</t>
   </si>
   <si>
     <t xml:space="preserve">VARCHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#contraints:maxLength</t>
   </si>
   <si>
     <t xml:space="preserve">boolean</t>
@@ -382,10 +391,10 @@
   <dimension ref="A1:G1019"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="21.9"/>
@@ -745,8 +754,8 @@
         <v>32</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="4" t="n">
-        <v>18</v>
+      <c r="D21" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>0</v>
@@ -760,16 +769,16 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G22" s="4" t="n">
         <v>6</v>
@@ -777,16 +786,16 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G23" s="4" t="n">
         <v>6</v>
@@ -794,16 +803,16 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G24" s="4" t="n">
         <v>8</v>
@@ -811,16 +820,16 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G25" s="4" t="n">
         <v>8</v>
@@ -828,20 +837,20 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="3" t="n">
-        <v>64</v>
-      </c>
-      <c r="E26" s="3" t="n">
-        <v>20</v>
+      <c r="D26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G26" s="3" t="n">
         <v>3</v>
@@ -849,18 +858,18 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="3" t="n">
-        <v>255</v>
+        <v>43</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G27" s="4" t="n">
         <v>12</v>
@@ -868,16 +877,16 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G28" s="4" t="n">
         <v>16</v>
@@ -885,16 +894,16 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G29" s="4" t="n">
         <v>16</v>
@@ -902,10 +911,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>36</v>
@@ -913,7 +922,7 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G30" s="4" t="n">
         <v>12</v>
@@ -921,10 +930,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>36</v>
@@ -932,7 +941,7 @@
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G31" s="4" t="n">
         <v>12</v>
@@ -940,10 +949,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>36</v>
@@ -951,7 +960,7 @@
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G32" s="4" t="n">
         <v>12</v>
@@ -959,10 +968,10 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>36</v>
@@ -970,7 +979,7 @@
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G33" s="4" t="n">
         <v>12</v>
@@ -978,10 +987,10 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>4095</v>
@@ -989,7 +998,7 @@
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G34" s="4" t="n">
         <v>12</v>

</xml_diff>

<commit_message>
JNG-2588: fix typo in excels and add parsing util to field.eol
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
@@ -121,7 +121,7 @@
     <t xml:space="preserve">DECIMAL</t>
   </si>
   <si>
-    <t xml:space="preserve">#contraints:precision</t>
+    <t xml:space="preserve">#constraints:precision</t>
   </si>
   <si>
     <t xml:space="preserve">float</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">java.math.BigDecimal</t>
   </si>
   <si>
-    <t xml:space="preserve">#contraints:scale</t>
+    <t xml:space="preserve">#constraints:scale</t>
   </si>
   <si>
     <t xml:space="preserve">java.lang.String</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">VARCHAR</t>
   </si>
   <si>
-    <t xml:space="preserve">#contraints:maxLength</t>
+    <t xml:space="preserve">#constraints:maxLength</t>
   </si>
   <si>
     <t xml:space="preserve">boolean</t>
@@ -391,10 +391,10 @@
   <dimension ref="A1:G1019"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="21.9"/>

</xml_diff>